<commit_message>
data excel masi ada yang salah kolom lat
</commit_message>
<xml_diff>
--- a/ml-service/Dataset_Wisata_Madura.xlsx
+++ b/ml-service/Dataset_Wisata_Madura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumen\Imam\Pribadi\SIB\Capstone\back-end\ml-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEB53D9-52D0-4EE4-9E50-4CEA713E0BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA1B8BC-8841-466E-97ED-01406827C336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>rating</t>
   </si>
   <si>
-    <t>Lat</t>
-  </si>
-  <si>
     <t>lon</t>
   </si>
   <si>
@@ -1254,6 +1251,9 @@
   </si>
   <si>
     <t>Parkir, Toilet, Kuliner, Tempat Ibadah</t>
+  </si>
+  <si>
+    <t>lat</t>
   </si>
 </sst>
 </file>
@@ -1579,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1631,10 +1631,10 @@
         <v>10</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -1648,13 +1648,13 @@
     </row>
     <row r="2" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="7">
         <v>0.33333333333333331</v>
@@ -1663,19 +1663,19 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="H2" s="8">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="K2" s="6">
         <v>-7.0562531760783296</v>
@@ -1695,13 +1695,13 @@
     </row>
     <row r="3" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>7</v>
@@ -1710,19 +1710,19 @@
         <v>7</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="H3" s="8">
         <v>0</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="6">
         <v>-7.1593806927427703</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="4" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="D4" s="7">
         <v>0.375</v>
@@ -1757,19 +1757,19 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="H4" s="8">
         <v>15000</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="K4" s="6">
         <v>-7.16032882308778</v>
@@ -1789,13 +1789,13 @@
     </row>
     <row r="5" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D5" s="7">
         <v>0</v>
@@ -1804,19 +1804,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="8">
         <v>0</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="K5" s="6">
         <v>-6.97275487235685</v>
@@ -1836,13 +1836,13 @@
     </row>
     <row r="6" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="7">
         <v>0</v>
@@ -1851,10 +1851,10 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -1863,7 +1863,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="6">
         <v>-6.9557206983162896</v>
@@ -1883,13 +1883,13 @@
     </row>
     <row r="7" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>7</v>
@@ -1898,19 +1898,19 @@
         <v>7</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="8">
         <v>10000</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="6">
         <v>-6.8848477296647799</v>
@@ -1930,13 +1930,13 @@
     </row>
     <row r="8" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>7</v>
@@ -1945,10 +1945,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="H8" s="8">
         <v>0</v>
@@ -1957,7 +1957,7 @@
         <v>7</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K8" s="6">
         <v>-7.0422093470048202</v>
@@ -1977,13 +1977,13 @@
     </row>
     <row r="9" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D9" s="7">
         <v>0.29166666666666669</v>
@@ -1992,10 +1992,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" s="8">
         <v>0</v>
@@ -2004,7 +2004,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" s="6">
         <v>-7.0200444155317099</v>
@@ -2024,13 +2024,13 @@
     </row>
     <row r="10" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>7</v>
@@ -2039,10 +2039,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="8">
         <v>0</v>
@@ -2051,7 +2051,7 @@
         <v>7</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K10" s="6">
         <v>-7.1104119914174104</v>
@@ -2071,13 +2071,13 @@
     </row>
     <row r="11" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>7</v>
@@ -2086,10 +2086,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="8">
         <v>0</v>
@@ -2098,7 +2098,7 @@
         <v>7</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K11" s="6">
         <v>-7.0262905809305298</v>
@@ -2118,13 +2118,13 @@
     </row>
     <row r="12" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="D12" s="7">
         <v>0.29166666666666669</v>
@@ -2133,19 +2133,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" s="8">
         <v>10000</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" s="6">
         <v>-6.8841857011571301</v>
@@ -2165,13 +2165,13 @@
     </row>
     <row r="13" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D13" s="7">
         <v>0</v>
@@ -2180,19 +2180,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="8">
         <v>10000</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K13" s="6">
         <v>-6.9852237321306498</v>
@@ -2212,13 +2212,13 @@
     </row>
     <row r="14" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="D14" s="7">
         <v>0.29166666666666669</v>
@@ -2227,19 +2227,19 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="H14" s="8">
         <v>0</v>
       </c>
       <c r="I14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="K14" s="6">
         <v>-6.8895568455788601</v>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="15" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>7</v>
@@ -2274,19 +2274,19 @@
         <v>7</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="8">
         <v>10000</v>
       </c>
       <c r="I15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="K15" s="6">
         <v>-6.8831003144336202</v>
@@ -2306,13 +2306,13 @@
     </row>
     <row r="16" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>7</v>
@@ -2321,10 +2321,10 @@
         <v>7</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="8">
         <v>0</v>
@@ -2333,7 +2333,7 @@
         <v>7</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K16" s="6">
         <v>-6.8931457743543003</v>
@@ -2353,13 +2353,13 @@
     </row>
     <row r="17" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D17" s="7">
         <v>0.29166666666666669</v>
@@ -2368,19 +2368,19 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H17" s="8">
         <v>5000</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K17" s="6">
         <v>-7.1587073075734597</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="18" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="D18" s="7">
         <v>0</v>
@@ -2415,10 +2415,10 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="8">
         <v>0</v>
@@ -2427,7 +2427,7 @@
         <v>7</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K18" s="6">
         <v>-7.1221859769528102</v>
@@ -2447,13 +2447,13 @@
     </row>
     <row r="19" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="D19" s="7">
         <v>0.29166666666666669</v>
@@ -2462,19 +2462,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="H19" s="8">
         <v>5000</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K19" s="6">
         <v>-7.0428586449504298</v>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="D20" s="7">
         <v>0.33333333333333331</v>
@@ -2509,19 +2509,19 @@
         <v>0.5</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H20" s="8">
         <v>0</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K20" s="6">
         <v>-7.0231358734565399</v>
@@ -2541,13 +2541,13 @@
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="D21" s="7">
         <v>0</v>
@@ -2556,19 +2556,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H21" s="8">
         <v>0</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="6">
         <v>-7.0400722493264398</v>
@@ -2588,13 +2588,13 @@
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
@@ -2603,19 +2603,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="8">
         <v>0</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K22" s="6">
         <v>-6.9485208776454499</v>
@@ -2635,13 +2635,13 @@
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="D23" s="7">
         <v>0</v>
@@ -2650,19 +2650,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="8">
         <v>0</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K23" s="6">
         <v>-7.0279255124262301</v>
@@ -2682,13 +2682,13 @@
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
@@ -2697,19 +2697,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H24" s="8">
         <v>0</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K24" s="6">
         <v>-7.15787248715153</v>
@@ -2729,13 +2729,13 @@
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
@@ -2744,19 +2744,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" s="8">
         <v>0</v>
       </c>
       <c r="I25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="K25" s="6">
         <v>-7.0410514919170302</v>
@@ -2776,13 +2776,13 @@
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="D26" s="7">
         <v>0.33333333333333331</v>
@@ -2791,19 +2791,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H26" s="8">
         <v>3000</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K26" s="6">
         <v>-7.0476693356659199</v>
@@ -2823,13 +2823,13 @@
     </row>
     <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="D27" s="7">
         <v>0.33333333333333331</v>
@@ -2838,10 +2838,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H27" s="8">
         <v>0</v>
@@ -2850,7 +2850,7 @@
         <v>7</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K27" s="6">
         <v>-7.0332183081351696</v>
@@ -2870,13 +2870,13 @@
     </row>
     <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="D28" s="7">
         <v>0</v>
@@ -2885,19 +2885,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H28" s="8">
         <v>5000</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K28" s="6">
         <v>-6.8823135728683003</v>
@@ -2917,13 +2917,13 @@
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>7</v>
@@ -2932,10 +2932,10 @@
         <v>7</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H29" s="8">
         <v>0</v>
@@ -2944,7 +2944,7 @@
         <v>7</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K29" s="6">
         <v>-6.8874765969752501</v>
@@ -2964,13 +2964,13 @@
     </row>
     <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>7</v>
@@ -2979,19 +2979,19 @@
         <v>7</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H30" s="8">
         <v>0</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K30" s="6">
         <v>-7.0129388689591803</v>
@@ -3011,13 +3011,13 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="D31" s="7">
         <v>0.33333333333333331</v>
@@ -3026,19 +3026,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H31" s="8">
         <v>0</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K31" s="6">
         <v>-7.1552278232812503</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="D32" s="7">
         <v>0</v>
@@ -3073,19 +3073,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H32" s="8">
         <v>0</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K32" s="6">
         <v>-7.0435006144455201</v>
@@ -3105,13 +3105,13 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="D33" s="7">
         <v>0.25</v>
@@ -3120,19 +3120,19 @@
         <v>0.75</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H33" s="8">
         <v>5000</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K33" s="6">
         <v>-6.8923677864814401</v>
@@ -3152,13 +3152,13 @@
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="D34" s="7">
         <v>0</v>
@@ -3167,19 +3167,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H34" s="8">
         <v>5000</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K34" s="6">
         <v>-7.1945282838153899</v>
@@ -3199,13 +3199,13 @@
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="D35" s="7">
         <v>0.25</v>
@@ -3214,19 +3214,19 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H35" s="8">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K35" s="6">
         <v>-6.8974157393115201</v>
@@ -3246,13 +3246,13 @@
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>154</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>155</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>7</v>
@@ -3261,19 +3261,19 @@
         <v>7</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H36" s="8">
         <v>10000</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K36" s="6">
         <v>-7.3076045456303298</v>
@@ -3293,13 +3293,13 @@
     </row>
     <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>158</v>
       </c>
       <c r="D37" s="7">
         <v>0</v>
@@ -3308,19 +3308,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H37" s="8">
         <v>10000</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K37" s="6">
         <v>-7.2180957699475101</v>
@@ -3340,13 +3340,13 @@
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="D38" s="7">
         <v>0.3125</v>
@@ -3355,19 +3355,19 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H38" s="8">
         <v>10000</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K38" s="6">
         <v>-6.8887427342836398</v>
@@ -3387,13 +3387,13 @@
     </row>
     <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>166</v>
       </c>
       <c r="D39" s="7">
         <v>0.375</v>
@@ -3402,19 +3402,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H39" s="8">
         <v>0</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K39" s="6">
         <v>-7.1069186227886503</v>
@@ -3434,13 +3434,13 @@
     </row>
     <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>7</v>
@@ -3449,10 +3449,10 @@
         <v>7</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H40" s="8">
         <v>0</v>
@@ -3461,7 +3461,7 @@
         <v>7</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K40" s="6">
         <v>-7.2090514543004396</v>
@@ -3481,13 +3481,13 @@
     </row>
     <row r="41" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="D41" s="7">
         <v>0</v>
@@ -3496,19 +3496,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H41" s="8">
         <v>0</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K41" s="6">
         <v>-7.2082701422971098</v>
@@ -3528,13 +3528,13 @@
     </row>
     <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>177</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>7</v>
@@ -3543,19 +3543,19 @@
         <v>7</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H42" s="8">
         <v>0</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K42" s="6">
         <v>-7.1930537401677501</v>
@@ -3575,13 +3575,13 @@
     </row>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>7</v>
@@ -3590,19 +3590,19 @@
         <v>7</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H43" s="8">
         <v>0</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K43" s="6">
         <v>-6.8859530486375498</v>
@@ -3622,13 +3622,13 @@
     </row>
     <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>185</v>
       </c>
       <c r="D44" s="7">
         <v>0.33333333333333331</v>
@@ -3637,19 +3637,19 @@
         <v>0.6875</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H44" s="8">
         <v>0</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K44" s="6">
         <v>-6.9126175541528303</v>
@@ -3669,13 +3669,13 @@
     </row>
     <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="D45" s="7">
         <v>0.33333333333333331</v>
@@ -3684,19 +3684,19 @@
         <v>0.875</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H45" s="8">
         <v>0</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K45" s="6">
         <v>-7.1916661336380301</v>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="D46" s="7">
         <v>0.33333333333333331</v>
@@ -3731,10 +3731,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F46" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G46" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="H46" s="8">
         <v>0</v>
@@ -3743,7 +3743,7 @@
         <v>7</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K46" s="6">
         <v>-6.8966708003211199</v>
@@ -3763,13 +3763,13 @@
     </row>
     <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>194</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="D47" s="7">
         <v>0</v>
@@ -3778,19 +3778,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H47" s="8">
         <v>0</v>
       </c>
       <c r="I47" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="J47" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="J47" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="K47" s="6">
         <v>-6.9120880608692197</v>
@@ -3810,13 +3810,13 @@
     </row>
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="D48" s="7">
         <v>0.33333333333333331</v>
@@ -3825,19 +3825,19 @@
         <v>0</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H48" s="8">
         <v>0</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K48" s="6">
         <v>-7.1916775824052701</v>
@@ -3857,13 +3857,13 @@
     </row>
     <row r="49" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>202</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>203</v>
       </c>
       <c r="D49" s="7">
         <v>0.29166666666666669</v>
@@ -3872,19 +3872,19 @@
         <v>0.6875</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H49" s="8">
         <v>0</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K49" s="6">
         <v>-7.1907955594338997</v>
@@ -3904,13 +3904,13 @@
     </row>
     <row r="50" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>207</v>
       </c>
       <c r="D50" s="7">
         <v>0.33333333333333331</v>
@@ -3919,19 +3919,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H50" s="8">
         <v>0</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K50" s="6">
         <v>-7.1960907913387802</v>
@@ -3951,13 +3951,13 @@
     </row>
     <row r="51" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>209</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>210</v>
       </c>
       <c r="D51" s="7">
         <v>0</v>
@@ -3966,10 +3966,10 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H51" s="8">
         <v>0</v>
@@ -3978,7 +3978,7 @@
         <v>7</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K51" s="6">
         <v>-7.2198290456833796</v>
@@ -3998,13 +3998,13 @@
     </row>
     <row r="52" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>213</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>7</v>
@@ -4013,19 +4013,19 @@
         <v>7</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H52" s="8">
         <v>0</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K52" s="6">
         <v>-6.8919108951761396</v>
@@ -4045,13 +4045,13 @@
     </row>
     <row r="53" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>216</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>217</v>
       </c>
       <c r="D53" s="7">
         <v>0.3125</v>
@@ -4060,19 +4060,19 @@
         <v>0.6875</v>
       </c>
       <c r="F53" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="H53" s="8">
         <v>25000</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K53" s="6">
         <v>-7.1938813677752904</v>
@@ -4092,13 +4092,13 @@
     </row>
     <row r="54" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="C54" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>222</v>
       </c>
       <c r="D54" s="7">
         <v>0</v>
@@ -4107,19 +4107,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H54" s="8">
         <v>0</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K54" s="6">
         <v>-7.2048084605951397</v>
@@ -4139,13 +4139,13 @@
     </row>
     <row r="55" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>225</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>226</v>
       </c>
       <c r="D55" s="7">
         <v>0.22916666666666666</v>
@@ -4154,19 +4154,19 @@
         <v>0.75</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H55" s="8">
         <v>5000</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K55" s="6">
         <v>-7.1648457439274704</v>
@@ -4186,13 +4186,13 @@
     </row>
     <row r="56" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>230</v>
       </c>
       <c r="D56" s="7">
         <v>0.20833333333333334</v>
@@ -4201,19 +4201,19 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H56" s="8">
         <v>2000</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K56" s="6">
         <v>-7.2331874095648798</v>
@@ -4233,13 +4233,13 @@
     </row>
     <row r="57" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" s="10" t="s">
         <v>233</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>234</v>
       </c>
       <c r="D57" s="7">
         <v>0.29166666666666669</v>
@@ -4248,19 +4248,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H57" s="8">
         <v>2000</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K57" s="6">
         <v>-7.1372637816611704</v>
@@ -4280,13 +4280,13 @@
     </row>
     <row r="58" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="D58" s="7">
         <v>0.29166666666666669</v>
@@ -4295,19 +4295,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H58" s="8">
         <v>0</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K58" s="6">
         <v>-7.25049906568014</v>
@@ -4327,13 +4327,13 @@
     </row>
     <row r="59" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>240</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>241</v>
       </c>
       <c r="D59" s="7">
         <v>0.25</v>
@@ -4342,19 +4342,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H59" s="8">
         <v>5000</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K59" s="6">
         <v>-7.0764782339138197</v>
@@ -4374,13 +4374,13 @@
     </row>
     <row r="60" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="D60" s="7">
         <v>0</v>
@@ -4389,19 +4389,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H60" s="8">
         <v>3000</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K60" s="6">
         <v>-7.1794255086479</v>
@@ -4421,13 +4421,13 @@
     </row>
     <row r="61" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" s="10" t="s">
         <v>248</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>249</v>
       </c>
       <c r="D61" s="7">
         <v>0.29166666666666669</v>
@@ -4436,19 +4436,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H61" s="8">
         <v>5000</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K61" s="6">
         <v>-7.0226766047011804</v>
@@ -4468,13 +4468,13 @@
     </row>
     <row r="62" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C62" s="10" t="s">
         <v>252</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>253</v>
       </c>
       <c r="D62" s="7">
         <v>0.33333333333333331</v>
@@ -4483,19 +4483,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H62" s="8">
         <v>10000</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K62" s="6">
         <v>-7.1104318419558101</v>
@@ -4515,13 +4515,13 @@
     </row>
     <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="D63" s="7">
         <v>0</v>
@@ -4530,19 +4530,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H63" s="8">
         <v>10000</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K63" s="6">
         <v>-7.0266986077407596</v>
@@ -4562,13 +4562,13 @@
     </row>
     <row r="64" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="D64" s="7">
         <v>0.29166666666666669</v>
@@ -4577,19 +4577,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H64" s="8">
         <v>5000</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K64" s="6">
         <v>-7.0497456251916102</v>
@@ -4609,13 +4609,13 @@
     </row>
     <row r="65" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>263</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="D65" s="7">
         <v>0.33333333333333331</v>
@@ -4624,19 +4624,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H65" s="8">
         <v>0</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K65" s="6">
         <v>-7.0979316704125504</v>
@@ -4656,13 +4656,13 @@
     </row>
     <row r="66" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C66" s="10" t="s">
         <v>267</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>268</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>7</v>
@@ -4671,19 +4671,19 @@
         <v>7</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H66" s="8">
         <v>0</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K66" s="6">
         <v>-7.1509583079350101</v>
@@ -4703,13 +4703,13 @@
     </row>
     <row r="67" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>270</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>271</v>
       </c>
       <c r="D67" s="7">
         <v>0.3125</v>
@@ -4718,19 +4718,19 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H67" s="8">
         <v>0</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K67" s="6">
         <v>-7.1597695479385397</v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="68" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>273</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>274</v>
       </c>
       <c r="D68" s="7">
         <v>0.29166666666666669</v>
@@ -4765,19 +4765,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H68" s="8">
         <v>5000</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K68" s="6">
         <v>-7.2062618978593402</v>
@@ -4797,13 +4797,13 @@
     </row>
     <row r="69" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>277</v>
       </c>
       <c r="D69" s="7">
         <v>0.33333333333333331</v>
@@ -4812,19 +4812,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H69" s="8">
         <v>0</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K69" s="6">
         <v>-7.1671868749746102</v>
@@ -4844,13 +4844,13 @@
     </row>
     <row r="70" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>282</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>7</v>
@@ -4859,19 +4859,19 @@
         <v>7</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H70" s="8">
         <v>10000</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J70" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K70" s="6">
         <v>-6.9831184000000004</v>
@@ -4891,13 +4891,13 @@
     </row>
     <row r="71" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>285</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="D71" s="7">
         <v>0</v>
@@ -4906,19 +4906,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H71" s="8">
         <v>25000</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J71" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K71" s="6">
         <v>-7.2014285999999998</v>
@@ -4938,13 +4938,13 @@
     </row>
     <row r="72" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="D72" s="7">
         <v>0.33333333333333331</v>
@@ -4953,19 +4953,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H72" s="8">
         <v>0</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K72" s="6">
         <v>-6.9957940000000001</v>
@@ -4985,13 +4985,13 @@
     </row>
     <row r="73" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>293</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>7</v>
@@ -5000,19 +5000,19 @@
         <v>7</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H73" s="8">
         <v>5000</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K73" s="6">
         <v>-7.0191901999999997</v>
@@ -5032,13 +5032,13 @@
     </row>
     <row r="74" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C74" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="D74" s="7">
         <v>0.33333333333333331</v>
@@ -5047,19 +5047,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H74" s="8">
         <v>15000</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K74" s="6">
         <v>-6.8982077000000004</v>
@@ -5079,13 +5079,13 @@
     </row>
     <row r="75" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C75" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>301</v>
       </c>
       <c r="D75" s="7">
         <v>0.29166666666666669</v>
@@ -5094,19 +5094,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H75" s="8">
         <v>10000</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K75" s="6">
         <v>-7.0934799999999996</v>
@@ -5126,13 +5126,13 @@
     </row>
     <row r="76" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C76" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="D76" s="7">
         <v>0</v>
@@ -5141,19 +5141,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H76" s="8">
         <v>20000</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K76" s="6">
         <v>-6.8791954000000004</v>
@@ -5173,13 +5173,13 @@
     </row>
     <row r="77" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>309</v>
       </c>
       <c r="D77" s="7">
         <v>0.33333333333333331</v>
@@ -5188,19 +5188,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H77" s="8">
         <v>5000</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J77" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K77" s="6">
         <v>-6.9178648000000003</v>
@@ -5220,13 +5220,13 @@
     </row>
     <row r="78" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C78" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="D78" s="7">
         <v>0</v>
@@ -5235,19 +5235,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H78" s="8">
         <v>5000</v>
       </c>
       <c r="I78" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J78" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K78" s="6">
         <v>-7.1751702999999996</v>
@@ -5267,13 +5267,13 @@
     </row>
     <row r="79" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C79" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>317</v>
       </c>
       <c r="D79" s="7">
         <v>0</v>
@@ -5282,19 +5282,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H79" s="8">
         <v>20000</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J79" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K79" s="6">
         <v>-6.8861093999999996</v>
@@ -5314,13 +5314,13 @@
     </row>
     <row r="80" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="D80" s="7">
         <v>0</v>
@@ -5329,19 +5329,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H80" s="8">
         <v>0</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J80" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K80" s="6">
         <v>-6.8703621999999998</v>
@@ -5361,13 +5361,13 @@
     </row>
     <row r="81" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>324</v>
       </c>
       <c r="D81" s="7">
         <v>0.29166666666666669</v>
@@ -5376,19 +5376,19 @@
         <v>0.875</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H81" s="8">
         <v>0</v>
       </c>
       <c r="I81" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J81" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K81" s="6">
         <v>-6.9705250000000003</v>
@@ -5408,13 +5408,13 @@
     </row>
     <row r="82" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C82" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="D82" s="7">
         <v>0.25</v>
@@ -5423,19 +5423,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H82" s="8">
         <v>10000</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K82" s="6">
         <v>-7.0789985</v>
@@ -5455,13 +5455,13 @@
     </row>
     <row r="83" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="D83" s="7">
         <v>0.20833333333333334</v>
@@ -5470,19 +5470,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H83" s="8">
         <v>10000</v>
       </c>
       <c r="I83" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K83" s="6">
         <v>-7.0108300999999997</v>
@@ -5502,13 +5502,13 @@
     </row>
     <row r="84" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>334</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>335</v>
       </c>
       <c r="D84" s="7">
         <v>0.29166666666666669</v>
@@ -5517,19 +5517,19 @@
         <v>0.91597222222222219</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H84" s="8">
         <v>10000</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K84" s="6">
         <v>-7.0152004999999997</v>
@@ -5549,13 +5549,13 @@
     </row>
     <row r="85" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>338</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>339</v>
       </c>
       <c r="D85" s="7">
         <v>0.29166666666666669</v>
@@ -5564,19 +5564,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H85" s="8">
         <v>10000</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K85" s="6">
         <v>-7.0141752000000004</v>
@@ -5596,13 +5596,13 @@
     </row>
     <row r="86" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>343</v>
       </c>
       <c r="D86" s="7">
         <v>0.33333333333333331</v>
@@ -5611,19 +5611,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H86" s="8">
         <v>0</v>
       </c>
       <c r="I86" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="J86" s="9" t="s">
         <v>344</v>
-      </c>
-      <c r="J86" s="9" t="s">
-        <v>345</v>
       </c>
       <c r="K86" s="6">
         <v>-6.9902442999999996</v>
@@ -5643,13 +5643,13 @@
     </row>
     <row r="87" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>347</v>
       </c>
       <c r="D87" s="7">
         <v>0.25</v>
@@ -5658,19 +5658,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H87" s="8">
         <v>5000</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K87" s="6">
         <v>-7.0071139000000002</v>
@@ -5690,13 +5690,13 @@
     </row>
     <row r="88" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="D88" s="7">
         <v>0</v>
@@ -5705,19 +5705,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H88" s="8">
         <v>0</v>
       </c>
       <c r="I88" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J88" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K88" s="6">
         <v>-7.0082554000000004</v>
@@ -5737,13 +5737,13 @@
     </row>
     <row r="89" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>353</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>354</v>
       </c>
       <c r="D89" s="7">
         <v>0</v>
@@ -5752,19 +5752,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H89" s="8">
         <v>10000</v>
       </c>
       <c r="I89" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K89" s="6">
         <v>-7.0280481999999997</v>
@@ -5784,13 +5784,13 @@
     </row>
     <row r="90" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>357</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>358</v>
       </c>
       <c r="D90" s="7">
         <v>0</v>
@@ -5799,19 +5799,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H90" s="8">
         <v>10000</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K90" s="6">
         <v>-6.9746915999999999</v>
@@ -5831,13 +5831,13 @@
     </row>
     <row r="91" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>360</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>361</v>
       </c>
       <c r="D91" s="7">
         <v>0</v>
@@ -5846,19 +5846,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H91" s="8">
         <v>10000</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J91" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K91" s="6">
         <v>-7.0460323999999996</v>
@@ -5878,13 +5878,13 @@
     </row>
     <row r="92" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>364</v>
       </c>
       <c r="D92" s="7">
         <v>0</v>
@@ -5893,19 +5893,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H92" s="8">
         <v>10000</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J92" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K92" s="6">
         <v>-6.9958302999999997</v>
@@ -5925,13 +5925,13 @@
     </row>
     <row r="93" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>367</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>368</v>
       </c>
       <c r="D93" s="7">
         <v>0</v>
@@ -5940,19 +5940,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H93" s="8">
         <v>10000</v>
       </c>
       <c r="I93" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K93" s="6">
         <v>-6.8858085000000004</v>
@@ -5972,13 +5972,13 @@
     </row>
     <row r="94" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>370</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>371</v>
       </c>
       <c r="D94" s="7">
         <v>0</v>
@@ -5987,19 +5987,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H94" s="8">
         <v>10000</v>
       </c>
       <c r="I94" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J94" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K94" s="6">
         <v>-7.0654506000000001</v>
@@ -6019,13 +6019,13 @@
     </row>
     <row r="95" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>373</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>374</v>
       </c>
       <c r="D95" s="7">
         <v>0</v>
@@ -6034,19 +6034,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H95" s="8">
         <v>10000</v>
       </c>
       <c r="I95" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K95" s="6">
         <v>-6.9966328000000004</v>
@@ -6066,13 +6066,13 @@
     </row>
     <row r="96" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>377</v>
       </c>
       <c r="D96" s="7">
         <v>0</v>
@@ -6081,19 +6081,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H96" s="8">
         <v>0</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K96" s="6">
         <v>-7.0080780999999996</v>
@@ -6113,13 +6113,13 @@
     </row>
     <row r="97" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>379</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>380</v>
       </c>
       <c r="D97" s="7">
         <v>0.29166666666666669</v>
@@ -6128,19 +6128,19 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H97" s="8">
         <v>15000</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K97" s="6">
         <v>-7.0081176000000003</v>
@@ -6160,13 +6160,13 @@
     </row>
     <row r="98" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>383</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>384</v>
       </c>
       <c r="D98" s="7">
         <v>0</v>
@@ -6175,19 +6175,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H98" s="8">
         <v>300000</v>
       </c>
       <c r="I98" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K98" s="6">
         <v>-6.9028644000000003</v>
@@ -6207,13 +6207,13 @@
     </row>
     <row r="99" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>388</v>
       </c>
       <c r="D99" s="7">
         <v>0</v>
@@ -6222,19 +6222,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H99" s="8">
         <v>5000</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J99" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K99" s="6">
         <v>-7.1205553999999998</v>
@@ -6254,13 +6254,13 @@
     </row>
     <row r="100" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C100" s="6" t="s">
         <v>391</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>392</v>
       </c>
       <c r="D100" s="7">
         <v>0</v>
@@ -6269,10 +6269,10 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H100" s="8">
         <v>0</v>
@@ -6281,7 +6281,7 @@
         <v>7</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K100" s="6">
         <v>-7.0456190999999997</v>
@@ -6301,13 +6301,13 @@
     </row>
     <row r="101" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>394</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>395</v>
       </c>
       <c r="D101" s="7">
         <v>0</v>
@@ -6316,19 +6316,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H101" s="8">
         <v>5000</v>
       </c>
       <c r="I101" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J101" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K101" s="6">
         <v>-6.9935248999999997</v>
@@ -6348,13 +6348,13 @@
     </row>
     <row r="102" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D102" s="7">
         <v>0</v>
@@ -6363,19 +6363,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H102" s="8">
         <v>0</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J102" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K102" s="6">
         <v>-7.1751702999999996</v>
@@ -6395,13 +6395,13 @@
     </row>
     <row r="103" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C103" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="D103" s="7">
         <v>0.29166666666666669</v>
@@ -6410,19 +6410,19 @@
         <v>0.875</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H103" s="8">
         <v>10000</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K103" s="6">
         <v>-7.1049290000000003</v>
@@ -6442,13 +6442,13 @@
     </row>
     <row r="104" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>405</v>
       </c>
       <c r="D104" s="7">
         <v>0.25</v>
@@ -6457,19 +6457,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H104" s="8">
         <v>10000</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K104" s="6">
         <v>-7.0077316999999999</v>

</xml_diff>

<commit_message>
nambahin link url images
</commit_message>
<xml_diff>
--- a/ml-service/Dataset_Wisata_Madura.xlsx
+++ b/ml-service/Dataset_Wisata_Madura.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumen\Imam\Pribadi\SIB\Capstone\back-end\ml-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8317D817-22B0-4A89-BA0A-044397778053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4293698-3904-4415-B5EA-9106D4C34285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="509">
   <si>
     <t>Agro Edu Wisata Kebun Bang Jani</t>
   </si>
@@ -1257,6 +1257,306 @@
   </si>
   <si>
     <t>visitor</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FAgro%20Edu%20Wisata%20Kebun%20Bang%20Jani.jpg?alt=media&amp;token=b972b187-6d8c-4e8f-a33d-f0ff239b6a26</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPantai%20Rindu.jpg?alt=media&amp;token=88ebc627-ff89-4704-941e-df5c1dbb7f33</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FWisata%20Alam%20Kesek.jpg?alt=media&amp;token=8e9eed16-da1d-46bb-9c5e-32a6741b867b</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPandela%20(Pantai%20Desa%20Lajing).jpg?alt=media&amp;token=9ac9f265-98f3-41ee-a6dd-3df0355b753c</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMakam%20Agung%20Arosbaya.jpg?alt=media&amp;token=8b6dc199-9eba-4e37-b3f5-ac8bc1c792fd</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPantai%20Biru.jpg?alt=media&amp;token=8551c0f9-c5e1-4615-80fd-067dcb8d1c14</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FApi%20Alam%20Konang.png?alt=media&amp;token=20fda9cc-7065-42af-89d8-bf4daa29b442</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FAir%20Terjun%20Kokop.jpg?alt=media&amp;token=438ea54d-5edf-47b0-a1c9-8e61e4da0e83</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FBukit%20Pendabah.jpeg?alt=media&amp;token=2a191061-c502-42e1-b365-0aefdf02117a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FGunung%20Geger.jpg?alt=media&amp;token=44087d33-1461-437c-a97d-2f4a8609d644</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FHutan%20Mangrove%20Labuhan.jpg?alt=media&amp;token=bb7f6c31-f93d-4f2b-aa37-f8d8e41b43e9</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPantai%20Gebang.jpg?alt=media&amp;token=09475c53-061b-46de-b396-894b2b5b0735</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FKampung%20Batik%20Paseseh.jpg?alt=media&amp;token=fd6ae440-68cc-4e87-9fb1-0135673f21b2</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPantai%20Siring%20Kemuning.png?alt=media&amp;token=65b89dd5-1822-46c5-b6e8-f2a68e605f9a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPantai%20Lobuk%20Bumi%20Anyar.png?alt=media&amp;token=ce8e6adf-5ba8-418c-8cfd-f03ba812b3c4</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FKutai%20Sukbar.jpg?alt=media&amp;token=1c6cfbb5-77d2-4eb5-b2e3-dd4387b9963e</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FTaman%20Rekreasi%20Kota%20Bangkalan.jpg?alt=media&amp;token=e1c6a57f-e4ce-4e62-8e8c-cd9f51354d8f</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FStadion%20Kerapan%20sapi%20R.P%20Moh%20Noer.jpg?alt=media&amp;token=56b224c2-7736-4eff-ba58-4b33f1fec653</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FKolla%20Langgundih.png?alt=media&amp;token=4716fdfb-8b4b-4305-9245-c823c03d39c0</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMakam%20Aer%20Mata%20Ebu.jpg?alt=media&amp;token=aa06dfc9-a300-4ad0-ac4f-f394cd74852c</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMakam%20Sultan%20Abdul%20Kadirun.jpg?alt=media&amp;token=b8aebc23-778f-4561-be56-6009023fe6d0</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMakam%20Sunan%20Cendana.jpg?alt=media&amp;token=a6fc7849-6cde-4d4a-9397-e773f9ffcb31</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMakam%20Syaikhona%20Kholil.jpeg?alt=media&amp;token=92209284-9a27-4097-ac65-2c74bf677002</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMuseum%20Bangkalan%20Cakraningrat.jpg?alt=media&amp;token=4f179d8d-0c28-4d27-9d44-7da5346c79a4</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMuseum%20Perusnia.jpeg?alt=media&amp;token=6c65c72e-80c0-4d6a-a52e-65fc625c679a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPantai%20Tlangoh.jpg?alt=media&amp;token=8c31902d-cc17-440d-be92-1d317b975e08</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPerahu%20Sarimuna.jpeg?alt=media&amp;token=a3cc69be-9752-44e1-b720-51f705ab2a1f</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FJembatan%20Harapan%20Bancaran.png?alt=media&amp;token=8a894c42-df5c-4ccd-97f3-06242a0b6f2f</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FGoa%20Petapa%20Beach.jpg?alt=media&amp;token=2cf30899-b97b-47a2-8002-437120a39958</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FKrahiga.png?alt=media&amp;token=bcbd514a-2212-4031-ac4f-18b4a98ba9b4</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FAir%20Terjun%20Toroan.jpg?alt=media&amp;token=b5a1f424-8e02-4f60-80fe-4703b12fea0b</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FGoa%20Lebar.jpg?alt=media&amp;token=1edbfbb4-68d6-418f-b31a-dcdfa84371f4</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FHutan%20Kera%20Nepa.jpg?alt=media&amp;token=21932d97-95fc-4df4-9c63-2bebf8c7db2c</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fkarang%20laut%20mandangin(2).JPG?alt=media&amp;token=f47b61de-d417-4bd6-b14f-199f790e3fd0</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20camplong.JPG?alt=media&amp;token=be4054d1-e9c0-4f1e-9b22-2650dc356f65</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20lon%20malang.JPG?alt=media&amp;token=1b2e09ba-c26e-4df6-aac2-94dc31b53463</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fwaduk%20klampis.JPG?alt=media&amp;token=6f0e1939-dce1-41a4-b544-2e5314411eb9</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fsumur%20tujuh%20panji%20laras.JPG?alt=media&amp;token=496870ad-33b1-4af9-b49b-2bb84376bd09</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fsitus%20ratu%20ibu.JPG?alt=media&amp;token=cffa1939-a546-4709-8ae8-411ded562157</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fsitus%20trunojoyo.JPG?alt=media&amp;token=b589db6b-ed39-47a7-a053-90e5279a7920</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FDesa%20Budaya%20Kerapan%20Sapi%20Ketapang%20Barat.JPG?alt=media&amp;token=6e730f20-214f-4aa7-a5fc-9b2aa5f367a1</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fdesa%20wisata%20petualangan%20panjat%20tebing%20margua.PNG?alt=media&amp;token=c9353ffd-cc07-4554-8f3e-8bf46f73d727</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmangrove%20sreseh.JPG?alt=media&amp;token=896e1328-2ca2-4a73-8dff-5dc13d59bd52</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fkampung%20tani%20panjalin.JPG?alt=media&amp;token=c7c16dfc-a3a9-470f-8e6a-203df1e273cd</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fkampong%20milon%20napote.JPG?alt=media&amp;token=b73c404b-88d7-4742-b942-6b66846c99e9</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FWMS%20Berung%20Ngambeng%20Spot%20Klobur.JPG?alt=media&amp;token=7f510ef7-5f73-4e83-9dbd-7ae88a647d2a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FTaman%20Wiyata%20Bahari%20Sampang.PNG?alt=media&amp;token=1dc70398-734e-4468-b371-b394a56c0019</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FPerpustakaan%20Dan%20Arsip%20Kota%20Sampang.jpg?alt=media&amp;token=4736cb8a-a801-4ff2-b347-bd1f6201c5a9</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20damar%20wulan.JPG?alt=media&amp;token=05f88ea5-0ad1-400c-977c-bbfa1ddd02dd</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FTaman%20Impian%20Desa%20Rabian.PNG?alt=media&amp;token=56f4d544-370e-4769-9ba6-75e6d613b61f</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fwater%20park%20sumekar.jpeg?alt=media&amp;token=3a4aa8da-d83d-44a3-9d61-37285881cfea</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fapi%20tak%20kunjung%20padam.JPG?alt=media&amp;token=ba0f0359-ecd7-40fa-8ae3-00ba9183b137</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmangrove%20lembung.JPG?alt=media&amp;token=3cda0349-c8c3-4d3e-8956-681f238fe2f3</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20jumiang.JPG?alt=media&amp;token=4656031a-131b-4130-9be5-34d3d02d8bf1</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20talang%20siring.JPG?alt=media&amp;token=bb49bd12-012d-4640-95cb-462c6f02890d</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20the%20legend%20pamekasan.jpg?alt=media&amp;token=2f87ab11-3c6e-41d6-9adb-d76da82143af</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fbukit%20kehi.JPG?alt=media&amp;token=d229ccc1-86f9-4028-87e9-c1ce64c4c065</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Feduwisata%20garam.JPG?alt=media&amp;token=10ce58a8-9569-4846-9aac-002b8409cbca</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fkampung%20durian%20pmksn.JPG?alt=media&amp;token=15680e51-6745-4178-8bc6-138471c39f40</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fkampung%20toron%20semalem.JPG?alt=media&amp;token=468ce9d9-0e1c-4bc7-9d09-0dd183a97b2a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpuncak%20ratu.JPG?alt=media&amp;token=56725887-c317-4b69-8343-7c306aaabba9</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fwisata%20sawah.JPG?alt=media&amp;token=e697e7df-6eec-46e2-8ee0-7b5695d05bed</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpesarean%20batu%20ampar.JPG?alt=media&amp;token=42b3129a-839a-4639-bf03-c528fd809fd9</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FMakam%20Ronggo%20Sukowati.JPG?alt=media&amp;token=d847b43c-33bc-46b2-bf74-79ce9ff73902</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmuseum%20mandhilaras.JPG?alt=media&amp;token=281e8794-8b97-4c15-8e37-467a6f3baa4d</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Ftaman%20edukasi%20_titik%20sejuta%20warna_.JPG?alt=media&amp;token=31c2c79b-ce77-49f3-a9ec-184247e41735</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FWisata%20Terpadu%20Bhurunan%20Murtajih.JPG?alt=media&amp;token=3b0e9c29-9292-428b-b638-293a6c733bc9</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FGili-Iyang.webp?alt=media&amp;token=287b1cb1-d0ae-4872-a197-bf3b96e9f35c</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fgili%20labak.jpeg?alt=media&amp;token=4df78c58-519d-4ffb-a32f-5c7005dec905</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fgoa-jeruk-.webp?alt=media&amp;token=0646b252-a472-4c2b-a439-45bdc67df6c2</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fgua%20payudan.jpeg?alt=media&amp;token=828c9689-a4bb-4cc8-9f90-0c7f605b119b</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fgoa%20soekarno.jpeg?alt=media&amp;token=ee32944d-a4cd-4400-ac57-36c4cc15f647</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmangrove%20kedatim.jpeg?alt=media&amp;token=730bdca0-6402-4c77-9099-509936d1b6fa</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20badur.jpeg?alt=media&amp;token=3afd679d-44e4-49be-ab32-251608288160</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20lombang.jpeg?alt=media&amp;token=e0f67109-bfa4-4ada-a91d-d1141155e5da</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20sembilan.jpeg?alt=media&amp;token=8ccea1de-e171-44fc-8750-468f0ff28c44</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20slopeng.jpeg?alt=media&amp;token=712b47c1-5b59-48e5-8986-0abe02d6d72e</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fwisata%20batu%20putih.jpeg?alt=media&amp;token=2a515026-5927-48a7-b64f-a3605b7655a3</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fwisata%20bukit%20kalompek.jpeg?alt=media&amp;token=73a10a25-cc01-4e7f-a028-5e3922484948</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Ftelaga%20kirmata.jpeg?alt=media&amp;token=b8ca07e6-0619-4354-b7b6-1232af7fa424</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmutiara%20tirta.jpeg?alt=media&amp;token=6ef3e2bb-2c77-44fc-8b4b-2579d027752f</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Ftaman%20tectona.jpeg?alt=media&amp;token=57546c84-5b22-4247-9034-64793f174f58</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Ftirta%20sumekar%20indah.jpeg?alt=media&amp;token=8c3e59e1-4d2d-4893-bec5-630960a7a4d1</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fwisata%20bukit%20tinggi%20daramista.jpeg?alt=media&amp;token=ae6054e5-6c1a-4264-9a3e-6b769d8299e6</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Ftaman%20kota%20adipura.jpeg?alt=media&amp;token=4eade221-54e7-4286-b644-7ee431b18361</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fasta%20gumuk%20kertasada.jpeg?alt=media&amp;token=3e66f717-b07a-430f-9376-0696fae65a2a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fasta%20joko%20tole.jpeg?alt=media&amp;token=f66fe5b2-2f82-4e3d-8b97-97fd7286b449</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fasta%20k%20faqih.jpeg?alt=media&amp;token=832e77e1-d0a1-4ab8-923f-f524e7651e6a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fasta%20katandur.jpeg?alt=media&amp;token=c2b5be88-e817-4bce-88cf-64c14cbb3811</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fasta%20panaongan.jpeg?alt=media&amp;token=e72135b1-36d8-4da1-94e2-36406ec4f112</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fasta%20sayyid%20yusuf.jpeg?alt=media&amp;token=2e181e1a-b9f3-4bde-a713-24615e6f070f</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmakam%20asta%20tinggi.jpeg?alt=media&amp;token=fb464c44-c813-4156-8bef-69cfe7f4e176</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmasjid%20jami%20sumenep.jpeg?alt=media&amp;token=530940e8-d7d9-422c-99c3-69e1d687dc8e</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fmuseum%20keraton.jpeg?alt=media&amp;token=6886f735-71d5-4c0e-b639-be7718b118f7</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Frumah%20kasur%20pasir.jpeg?alt=media&amp;token=e10e0ac2-8bd6-4e8f-b70e-dec0de7ae4c1</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FSitus%20Batugong.jpg?alt=media&amp;token=f5952726-05af-44a3-b30f-9e051f83d8fc</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20keris.jpeg?alt=media&amp;token=0f915461-f9dc-40cb-8947-266318da7091</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20sembilan%20gili%20genting.jpeg?alt=media&amp;token=008da410-c2c6-46e3-83ce-c83d718b6cf3</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2Fpantai%20e%20kaoghi.jpeg?alt=media&amp;token=3a722f97-b497-4e0e-8b41-b50907e3f87b</t>
+  </si>
+  <si>
+    <t>imageURL</t>
   </si>
 </sst>
 </file>
@@ -1303,7 +1603,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1326,11 +1626,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1362,19 +1727,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1592,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1611,47 +1996,51 @@
     <col min="11" max="11" width="6.109375" customWidth="1"/>
     <col min="12" max="12" width="39.88671875" customWidth="1"/>
     <col min="13" max="13" width="22.88671875" customWidth="1"/>
+    <col min="14" max="14" width="184.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="20" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="20" t="s">
         <v>398</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="20" t="s">
         <v>400</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="21" t="s">
         <v>403</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="22" t="s">
         <v>405</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="23" t="s">
         <v>407</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>508</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1664,44 +2053,47 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="15">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="15">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="14">
         <v>2342</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="16">
         <v>0</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="14">
         <v>-7.0562531760783296</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="18">
         <v>112.777121217306</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>409</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1750,8 +2142,11 @@
       <c r="L3" s="6">
         <v>-7.1593806927427703</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="11">
         <v>112.776644379763</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>410</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1800,8 +2195,11 @@
       <c r="L4" s="6">
         <v>-7.16032882308778</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="11">
         <v>112.77219060489099</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>411</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1850,8 +2248,11 @@
       <c r="L5" s="6">
         <v>-6.97275487235685</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="11">
         <v>112.79423657976299</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>412</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1900,8 +2301,11 @@
       <c r="L6" s="6">
         <v>-6.9557206983162896</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="11">
         <v>112.84774550030301</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>413</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1950,8 +2354,11 @@
       <c r="L7" s="6">
         <v>-6.8848477296647799</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="11">
         <v>113.079132550927</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>414</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -2000,8 +2407,11 @@
       <c r="L8" s="6">
         <v>-7.0422093470048202</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="11">
         <v>113.073687635062</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>415</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -2050,8 +2460,11 @@
       <c r="L9" s="6">
         <v>-7.0200444155317099</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="11">
         <v>113.121777195108</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>416</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -2100,8 +2513,11 @@
       <c r="L10" s="6">
         <v>-7.1104119914174104</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="11">
         <v>112.744883418382</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>417</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -2150,8 +2566,11 @@
       <c r="L11" s="6">
         <v>-7.0262905809305298</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="11">
         <v>112.932690819564</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>418</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -2200,8 +2619,11 @@
       <c r="L12" s="6">
         <v>-6.8841857011571301</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="11">
         <v>112.99368480591799</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>419</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -2250,8 +2672,11 @@
       <c r="L13" s="6">
         <v>-6.9852237321306498</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="11">
         <v>112.78677076441799</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>420</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -2300,8 +2725,11 @@
       <c r="L14" s="6">
         <v>-6.8895568455788601</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="11">
         <v>113.085181550927</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>421</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -2350,8 +2778,11 @@
       <c r="L15" s="6">
         <v>-6.8831003144336202</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="11">
         <v>113.05564733062999</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>422</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -2400,8 +2831,11 @@
       <c r="L16" s="6">
         <v>-6.8931457743543003</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="11">
         <v>113.124476949129</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>423</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -2450,8 +2884,11 @@
       <c r="L17" s="6">
         <v>-7.1587073075734597</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="11">
         <v>112.79461308532601</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>424</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -2500,8 +2937,11 @@
       <c r="L18" s="6">
         <v>-7.1221859769528102</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="11">
         <v>112.813400050927</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>424</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -2550,8 +2990,11 @@
       <c r="L19" s="6">
         <v>-7.0428586449504298</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="11">
         <v>112.740382704891</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -2600,8 +3043,11 @@
       <c r="L20" s="6">
         <v>-7.0231358734565399</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="11">
         <v>112.761744479763</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -2650,8 +3096,11 @@
       <c r="L21" s="6">
         <v>-7.0400722493264398</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="11">
         <v>112.708753393254</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>427</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -2700,8 +3149,11 @@
       <c r="L22" s="6">
         <v>-6.9485208776454499</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="11">
         <v>112.856369483858</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>428</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -2750,8 +3202,11 @@
       <c r="L23" s="6">
         <v>-7.0279255124262301</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="11">
         <v>112.746339563907</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>429</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2800,8 +3255,11 @@
       <c r="L24" s="6">
         <v>-7.15787248715153</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24" s="11">
         <v>112.854163249072</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>430</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -2850,8 +3308,11 @@
       <c r="L25" s="6">
         <v>-7.0410514919170302</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25" s="11">
         <v>112.723478968126</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -2900,8 +3361,11 @@
       <c r="L26" s="6">
         <v>-7.0476693356659199</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26" s="11">
         <v>112.735317818382</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>432</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -2950,8 +3414,11 @@
       <c r="L27" s="6">
         <v>-7.0332183081351696</v>
       </c>
-      <c r="M27" s="6">
+      <c r="M27" s="11">
         <v>112.742761389035</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>433</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -3000,8 +3467,11 @@
       <c r="L28" s="6">
         <v>-6.8823135728683003</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M28" s="11">
         <v>113.047831479763</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>434</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -3050,8 +3520,11 @@
       <c r="L29" s="6">
         <v>-6.8874765969752501</v>
       </c>
-      <c r="M29" s="6">
+      <c r="M29" s="11">
         <v>113.082814502567</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>435</v>
       </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -3100,8 +3573,11 @@
       <c r="L30" s="6">
         <v>-7.0129388689591803</v>
       </c>
-      <c r="M30" s="6">
+      <c r="M30" s="11">
         <v>112.76106740438</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>436</v>
       </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -3150,8 +3626,11 @@
       <c r="L31" s="6">
         <v>-7.1552278232812503</v>
       </c>
-      <c r="M31" s="6">
+      <c r="M31" s="11">
         <v>112.802748917024</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>437</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -3200,8 +3679,11 @@
       <c r="L32" s="6">
         <v>-7.0435006144455201</v>
       </c>
-      <c r="M32" s="6">
+      <c r="M32" s="11">
         <v>112.70813719316401</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>438</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -3250,8 +3732,11 @@
       <c r="L33" s="6">
         <v>-6.8923677864814401</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M33" s="11">
         <v>113.312382208599</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>439</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -3300,8 +3785,11 @@
       <c r="L34" s="6">
         <v>-7.1945282838153899</v>
       </c>
-      <c r="M34" s="6">
+      <c r="M34" s="11">
         <v>113.255516320236</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>440</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -3350,8 +3838,11 @@
       <c r="L35" s="6">
         <v>-6.8974157393115201</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M35" s="11">
         <v>113.20085487925201</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>441</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -3400,8 +3891,11 @@
       <c r="L36" s="6">
         <v>-7.3076045456303298</v>
       </c>
-      <c r="M36" s="6">
+      <c r="M36" s="11">
         <v>113.211343279761</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>442</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -3450,8 +3944,11 @@
       <c r="L37" s="6">
         <v>-7.2180957699475101</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="11">
         <v>113.31936688279001</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -3500,8 +3997,11 @@
       <c r="L38" s="6">
         <v>-6.8887427342836398</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="11">
         <v>113.395441733052</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>444</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -3550,8 +4050,11 @@
       <c r="L39" s="6">
         <v>-7.1069186227886503</v>
       </c>
-      <c r="M39" s="6">
+      <c r="M39" s="11">
         <v>113.226025777722</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>445</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -3600,8 +4103,11 @@
       <c r="L40" s="6">
         <v>-7.2090514543004396</v>
       </c>
-      <c r="M40" s="6">
+      <c r="M40" s="11">
         <v>113.234600722748</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>446</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -3650,8 +4156,11 @@
       <c r="L41" s="6">
         <v>-7.2082701422971098</v>
       </c>
-      <c r="M41" s="6">
+      <c r="M41" s="11">
         <v>113.23283781532901</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>447</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -3700,8 +4209,11 @@
       <c r="L42" s="6">
         <v>-7.1930537401677501</v>
       </c>
-      <c r="M42" s="6">
+      <c r="M42" s="11">
         <v>113.25517002687801</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>448</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -3750,8 +4262,11 @@
       <c r="L43" s="6">
         <v>-6.8859530486375498</v>
       </c>
-      <c r="M43" s="6">
+      <c r="M43" s="11">
         <v>113.32147044202701</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>449</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -3800,8 +4315,11 @@
       <c r="L44" s="6">
         <v>-6.9126175541528303</v>
       </c>
-      <c r="M44" s="6">
+      <c r="M44" s="11">
         <v>113.476391501834</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>450</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -3850,8 +4368,11 @@
       <c r="L45" s="6">
         <v>-7.1916661336380301</v>
       </c>
-      <c r="M45" s="6">
+      <c r="M45" s="11">
         <v>113.088863874995</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>451</v>
       </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -3900,8 +4421,11 @@
       <c r="L46" s="6">
         <v>-6.8966708003211199</v>
       </c>
-      <c r="M46" s="6">
+      <c r="M46" s="11">
         <v>113.43771316158499</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>452</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -3950,8 +4474,11 @@
       <c r="L47" s="6">
         <v>-6.9120880608692197</v>
       </c>
-      <c r="M47" s="6">
+      <c r="M47" s="11">
         <v>113.39581961494</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>453</v>
       </c>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
@@ -4000,8 +4527,11 @@
       <c r="L48" s="6">
         <v>-7.1916775824052701</v>
       </c>
-      <c r="M48" s="6">
+      <c r="M48" s="11">
         <v>113.08835591718</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>454</v>
       </c>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
@@ -4050,8 +4580,11 @@
       <c r="L49" s="6">
         <v>-7.1907955594338997</v>
       </c>
-      <c r="M49" s="6">
+      <c r="M49" s="11">
         <v>113.25409771162499</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>455</v>
       </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -4100,8 +4633,11 @@
       <c r="L50" s="6">
         <v>-7.1960907913387802</v>
       </c>
-      <c r="M50" s="6">
+      <c r="M50" s="11">
         <v>113.25231035171301</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>456</v>
       </c>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
@@ -4150,8 +4686,11 @@
       <c r="L51" s="6">
         <v>-7.2198290456833796</v>
       </c>
-      <c r="M51" s="6">
+      <c r="M51" s="11">
         <v>113.22260685950801</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>457</v>
       </c>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
@@ -4200,8 +4739,11 @@
       <c r="L52" s="6">
         <v>-6.8919108951761396</v>
       </c>
-      <c r="M52" s="6">
+      <c r="M52" s="11">
         <v>113.261527707388</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>458</v>
       </c>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -4250,8 +4792,11 @@
       <c r="L53" s="6">
         <v>-7.1938813677752904</v>
       </c>
-      <c r="M53" s="6">
+      <c r="M53" s="11">
         <v>113.25779884615901</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>459</v>
       </c>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -4300,8 +4845,11 @@
       <c r="L54" s="6">
         <v>-7.2048084605951397</v>
       </c>
-      <c r="M54" s="6">
+      <c r="M54" s="11">
         <v>113.461667820776</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>460</v>
       </c>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -4350,8 +4898,11 @@
       <c r="L55" s="6">
         <v>-7.1648457439274704</v>
       </c>
-      <c r="M55" s="6">
+      <c r="M55" s="11">
         <v>113.575732834647</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>461</v>
       </c>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
@@ -4400,8 +4951,11 @@
       <c r="L56" s="6">
         <v>-7.2331874095648798</v>
       </c>
-      <c r="M56" s="6">
+      <c r="M56" s="11">
         <v>113.549338690422</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>462</v>
       </c>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
@@ -4450,8 +5004,11 @@
       <c r="L57" s="6">
         <v>-7.1372637816611704</v>
       </c>
-      <c r="M57" s="6">
+      <c r="M57" s="11">
         <v>113.59076589339401</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>463</v>
       </c>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
@@ -4500,8 +5057,11 @@
       <c r="L58" s="6">
         <v>-7.25049906568014</v>
       </c>
-      <c r="M58" s="6">
+      <c r="M58" s="11">
         <v>113.517067326709</v>
+      </c>
+      <c r="N58" s="12" t="s">
+        <v>464</v>
       </c>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
@@ -4550,8 +5110,11 @@
       <c r="L59" s="6">
         <v>-7.0764782339138197</v>
       </c>
-      <c r="M59" s="6">
+      <c r="M59" s="11">
         <v>113.610326834647</v>
+      </c>
+      <c r="N59" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
@@ -4600,8 +5163,11 @@
       <c r="L60" s="6">
         <v>-7.1794255086479</v>
       </c>
-      <c r="M60" s="6">
+      <c r="M60" s="11">
         <v>113.536004573079</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
@@ -4650,8 +5216,11 @@
       <c r="L61" s="6">
         <v>-7.0226766047011804</v>
       </c>
-      <c r="M61" s="6">
+      <c r="M61" s="11">
         <v>113.504072387571</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>467</v>
       </c>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
@@ -4700,8 +5269,11 @@
       <c r="L62" s="6">
         <v>-7.1104318419558101</v>
       </c>
-      <c r="M62" s="6">
+      <c r="M62" s="11">
         <v>113.505373919303</v>
+      </c>
+      <c r="N62" s="12" t="s">
+        <v>468</v>
       </c>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
@@ -4750,8 +5322,11 @@
       <c r="L63" s="6">
         <v>-7.0266986077407596</v>
       </c>
-      <c r="M63" s="6">
+      <c r="M63" s="11">
         <v>113.492764615068</v>
+      </c>
+      <c r="N63" s="12" t="s">
+        <v>469</v>
       </c>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
@@ -4800,8 +5375,11 @@
       <c r="L64" s="6">
         <v>-7.0497456251916102</v>
       </c>
-      <c r="M64" s="6">
+      <c r="M64" s="11">
         <v>113.57837857539801</v>
+      </c>
+      <c r="N64" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
@@ -4850,8 +5428,11 @@
       <c r="L65" s="6">
         <v>-7.0979316704125504</v>
       </c>
-      <c r="M65" s="6">
+      <c r="M65" s="11">
         <v>113.376994115328</v>
+      </c>
+      <c r="N65" s="12" t="s">
+        <v>471</v>
       </c>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
@@ -4900,8 +5481,11 @@
       <c r="L66" s="6">
         <v>-7.1509583079350101</v>
       </c>
-      <c r="M66" s="6">
+      <c r="M66" s="11">
         <v>113.484780119031</v>
+      </c>
+      <c r="N66" s="12" t="s">
+        <v>472</v>
       </c>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
@@ -4950,8 +5534,11 @@
       <c r="L67" s="6">
         <v>-7.1597695479385397</v>
       </c>
-      <c r="M67" s="6">
+      <c r="M67" s="11">
         <v>113.48497353041201</v>
+      </c>
+      <c r="N67" s="12" t="s">
+        <v>473</v>
       </c>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
@@ -5000,8 +5587,11 @@
       <c r="L68" s="6">
         <v>-7.2062618978593402</v>
       </c>
-      <c r="M68" s="6">
+      <c r="M68" s="11">
         <v>113.517765421961</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>474</v>
       </c>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
@@ -5050,8 +5640,11 @@
       <c r="L69" s="6">
         <v>-7.1671868749746102</v>
       </c>
-      <c r="M69" s="6">
+      <c r="M69" s="11">
         <v>113.507964784381</v>
+      </c>
+      <c r="N69" s="12" t="s">
+        <v>475</v>
       </c>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
@@ -5100,8 +5693,11 @@
       <c r="L70" s="6">
         <v>-6.9831184000000004</v>
       </c>
-      <c r="M70" s="6">
+      <c r="M70" s="11">
         <v>114.1722603</v>
+      </c>
+      <c r="N70" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -5150,8 +5746,11 @@
       <c r="L71" s="6">
         <v>-7.2014285999999998</v>
       </c>
-      <c r="M71" s="6">
+      <c r="M71" s="11">
         <v>114.04570440000001</v>
+      </c>
+      <c r="N71" s="12" t="s">
+        <v>477</v>
       </c>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -5200,8 +5799,11 @@
       <c r="L72" s="6">
         <v>-6.9957940000000001</v>
       </c>
-      <c r="M72" s="6">
+      <c r="M72" s="11">
         <v>113.84937309999999</v>
+      </c>
+      <c r="N72" s="12" t="s">
+        <v>478</v>
       </c>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -5250,8 +5852,11 @@
       <c r="L73" s="6">
         <v>-7.0191901999999997</v>
       </c>
-      <c r="M73" s="6">
+      <c r="M73" s="11">
         <v>113.6185469</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>479</v>
       </c>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -5300,8 +5905,11 @@
       <c r="L74" s="6">
         <v>-6.8982077000000004</v>
       </c>
-      <c r="M74" s="6">
+      <c r="M74" s="11">
         <v>113.6567794</v>
+      </c>
+      <c r="N74" s="12" t="s">
+        <v>480</v>
       </c>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
@@ -5350,8 +5958,11 @@
       <c r="L75" s="6">
         <v>-7.0934799999999996</v>
       </c>
-      <c r="M75" s="6">
+      <c r="M75" s="11">
         <v>113.86192320000001</v>
+      </c>
+      <c r="N75" s="12" t="s">
+        <v>481</v>
       </c>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
@@ -5400,8 +6011,11 @@
       <c r="L76" s="6">
         <v>-6.8791954000000004</v>
       </c>
-      <c r="M76" s="6">
+      <c r="M76" s="11">
         <v>113.9732791</v>
+      </c>
+      <c r="N76" s="12" t="s">
+        <v>482</v>
       </c>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
@@ -5450,8 +6064,11 @@
       <c r="L77" s="6">
         <v>-6.9178648000000003</v>
       </c>
-      <c r="M77" s="6">
+      <c r="M77" s="11">
         <v>114.06506760000001</v>
+      </c>
+      <c r="N77" s="12" t="s">
+        <v>483</v>
       </c>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
@@ -5500,8 +6117,11 @@
       <c r="L78" s="6">
         <v>-7.1751702999999996</v>
       </c>
-      <c r="M78" s="6">
+      <c r="M78" s="11">
         <v>113.9218159</v>
+      </c>
+      <c r="N78" s="12" t="s">
+        <v>484</v>
       </c>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
@@ -5550,8 +6170,11 @@
       <c r="L79" s="6">
         <v>-6.8861093999999996</v>
       </c>
-      <c r="M79" s="6">
+      <c r="M79" s="11">
         <v>113.792343</v>
+      </c>
+      <c r="N79" s="12" t="s">
+        <v>485</v>
       </c>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
@@ -5600,8 +6223,11 @@
       <c r="L80" s="6">
         <v>-6.8703621999999998</v>
       </c>
-      <c r="M80" s="6">
+      <c r="M80" s="11">
         <v>113.9243001</v>
+      </c>
+      <c r="N80" s="12" t="s">
+        <v>486</v>
       </c>
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
@@ -5650,8 +6276,11 @@
       <c r="L81" s="6">
         <v>-6.9705250000000003</v>
       </c>
-      <c r="M81" s="6">
+      <c r="M81" s="11">
         <v>114.09578260000001</v>
+      </c>
+      <c r="N81" s="12" t="s">
+        <v>487</v>
       </c>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
@@ -5700,8 +6329,11 @@
       <c r="L82" s="6">
         <v>-7.0789985</v>
       </c>
-      <c r="M82" s="6">
+      <c r="M82" s="11">
         <v>113.8262843</v>
+      </c>
+      <c r="N82" s="12" t="s">
+        <v>488</v>
       </c>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
@@ -5750,8 +6382,11 @@
       <c r="L83" s="6">
         <v>-7.0108300999999997</v>
       </c>
-      <c r="M83" s="6">
+      <c r="M83" s="11">
         <v>113.8637779</v>
+      </c>
+      <c r="N83" s="12" t="s">
+        <v>489</v>
       </c>
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
@@ -5800,8 +6435,11 @@
       <c r="L84" s="6">
         <v>-7.0152004999999997</v>
       </c>
-      <c r="M84" s="6">
+      <c r="M84" s="11">
         <v>138.16391999999999</v>
+      </c>
+      <c r="N84" s="12" t="s">
+        <v>490</v>
       </c>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
@@ -5850,8 +6488,11 @@
       <c r="L85" s="6">
         <v>-7.0141752000000004</v>
       </c>
-      <c r="M85" s="6">
+      <c r="M85" s="11">
         <v>113.82199230000001</v>
+      </c>
+      <c r="N85" s="12" t="s">
+        <v>491</v>
       </c>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
@@ -5900,8 +6541,11 @@
       <c r="L86" s="6">
         <v>-6.9902442999999996</v>
       </c>
-      <c r="M86" s="6">
+      <c r="M86" s="11">
         <v>113.8408225</v>
+      </c>
+      <c r="N86" s="12" t="s">
+        <v>459</v>
       </c>
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
@@ -5950,8 +6594,11 @@
       <c r="L87" s="6">
         <v>-7.0071139000000002</v>
       </c>
-      <c r="M87" s="6">
+      <c r="M87" s="11">
         <v>113.7999978</v>
+      </c>
+      <c r="N87" s="12" t="s">
+        <v>492</v>
       </c>
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
@@ -6000,8 +6647,11 @@
       <c r="L88" s="6">
         <v>-7.0082554000000004</v>
       </c>
-      <c r="M88" s="6">
+      <c r="M88" s="11">
         <v>113.8602317</v>
+      </c>
+      <c r="N88" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
@@ -6050,8 +6700,11 @@
       <c r="L89" s="6">
         <v>-7.0280481999999997</v>
       </c>
-      <c r="M89" s="6">
+      <c r="M89" s="11">
         <v>113.8956754</v>
+      </c>
+      <c r="N89" s="12" t="s">
+        <v>494</v>
       </c>
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
@@ -6100,8 +6753,11 @@
       <c r="L90" s="6">
         <v>-6.9746915999999999</v>
       </c>
-      <c r="M90" s="6">
+      <c r="M90" s="11">
         <v>113.91422420000001</v>
+      </c>
+      <c r="N90" s="12" t="s">
+        <v>495</v>
       </c>
       <c r="O90" s="1"/>
       <c r="P90" s="1"/>
@@ -6150,8 +6806,11 @@
       <c r="L91" s="6">
         <v>-7.0460323999999996</v>
       </c>
-      <c r="M91" s="6">
+      <c r="M91" s="11">
         <v>113.75626889999999</v>
+      </c>
+      <c r="N91" s="12" t="s">
+        <v>496</v>
       </c>
       <c r="O91" s="1"/>
       <c r="P91" s="1"/>
@@ -6200,8 +6859,11 @@
       <c r="L92" s="6">
         <v>-6.9958302999999997</v>
       </c>
-      <c r="M92" s="6">
+      <c r="M92" s="11">
         <v>113.8718064</v>
+      </c>
+      <c r="N92" s="12" t="s">
+        <v>497</v>
       </c>
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
@@ -6250,8 +6912,11 @@
       <c r="L93" s="6">
         <v>-6.8858085000000004</v>
       </c>
-      <c r="M93" s="6">
+      <c r="M93" s="11">
         <v>113.6614774</v>
+      </c>
+      <c r="N93" s="12" t="s">
+        <v>498</v>
       </c>
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
@@ -6300,8 +6965,11 @@
       <c r="L94" s="6">
         <v>-7.0654506000000001</v>
       </c>
-      <c r="M94" s="6">
+      <c r="M94" s="11">
         <v>113.9424303</v>
+      </c>
+      <c r="N94" s="12" t="s">
+        <v>499</v>
       </c>
       <c r="O94" s="1"/>
       <c r="P94" s="1"/>
@@ -6350,8 +7018,11 @@
       <c r="L95" s="6">
         <v>-6.9966328000000004</v>
       </c>
-      <c r="M95" s="6">
+      <c r="M95" s="11">
         <v>113.8435034</v>
+      </c>
+      <c r="N95" s="12" t="s">
+        <v>500</v>
       </c>
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
@@ -6400,8 +7071,11 @@
       <c r="L96" s="6">
         <v>-7.0080780999999996</v>
       </c>
-      <c r="M96" s="6">
+      <c r="M96" s="11">
         <v>113.85922789999999</v>
+      </c>
+      <c r="N96" s="12" t="s">
+        <v>501</v>
       </c>
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
@@ -6450,8 +7124,11 @@
       <c r="L97" s="6">
         <v>-7.0081176000000003</v>
       </c>
-      <c r="M97" s="6">
+      <c r="M97" s="11">
         <v>113.8628659</v>
+      </c>
+      <c r="N97" s="12" t="s">
+        <v>502</v>
       </c>
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
@@ -6500,8 +7177,11 @@
       <c r="L98" s="6">
         <v>-6.9028644000000003</v>
       </c>
-      <c r="M98" s="6">
+      <c r="M98" s="11">
         <v>114.02179</v>
+      </c>
+      <c r="N98" s="12" t="s">
+        <v>503</v>
       </c>
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
@@ -6550,8 +7230,11 @@
       <c r="L99" s="6">
         <v>-7.1205553999999998</v>
       </c>
-      <c r="M99" s="6">
+      <c r="M99" s="11">
         <v>114.33305559999999</v>
+      </c>
+      <c r="N99" s="12" t="s">
+        <v>504</v>
       </c>
       <c r="O99" s="1"/>
       <c r="P99" s="1"/>
@@ -6600,8 +7283,11 @@
       <c r="L100" s="6">
         <v>-7.0456190999999997</v>
       </c>
-      <c r="M100" s="6">
+      <c r="M100" s="11">
         <v>113.9593936</v>
+      </c>
+      <c r="N100" s="12" t="s">
+        <v>505</v>
       </c>
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
@@ -6650,8 +7336,11 @@
       <c r="L101" s="6">
         <v>-6.9935248999999997</v>
       </c>
-      <c r="M101" s="6">
+      <c r="M101" s="11">
         <v>114.1735705</v>
+      </c>
+      <c r="N101" s="12" t="s">
+        <v>505</v>
       </c>
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
@@ -6700,8 +7389,11 @@
       <c r="L102" s="6">
         <v>-7.1751702999999996</v>
       </c>
-      <c r="M102" s="6">
+      <c r="M102" s="11">
         <v>113.9218159</v>
+      </c>
+      <c r="N102" s="12" t="s">
+        <v>506</v>
       </c>
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
@@ -6750,8 +7442,11 @@
       <c r="L103" s="6">
         <v>-7.1049290000000003</v>
       </c>
-      <c r="M103" s="6">
+      <c r="M103" s="11">
         <v>113.88752839999999</v>
+      </c>
+      <c r="N103" s="12" t="s">
+        <v>507</v>
       </c>
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
@@ -6800,8 +7495,11 @@
       <c r="L104" s="6">
         <v>-7.0077316999999999</v>
       </c>
-      <c r="M104" s="6">
+      <c r="M104" s="11">
         <v>113.79997849999999</v>
+      </c>
+      <c r="N104" s="12" t="s">
+        <v>492</v>
       </c>
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>

</xml_diff>

<commit_message>
ada yang sama gambarnya, ganti link
</commit_message>
<xml_diff>
--- a/ml-service/Dataset_Wisata_Madura.xlsx
+++ b/ml-service/Dataset_Wisata_Madura.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumen\Imam\Pribadi\SIB\Capstone\back-end\ml-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4293698-3904-4415-B5EA-9106D4C34285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9A5D0A-5D9C-42A5-8219-AA023576227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="510">
   <si>
     <t>Agro Edu Wisata Kebun Bang Jani</t>
   </si>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>imageURL</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/newsmusic-b1986.appspot.com/o/kanto%2FTaman%20Bukit%20Anjhir.jpg?alt=media&amp;token=eaffa015-3564-4348-ab1d-9843eb5644c0</t>
   </si>
 </sst>
 </file>
@@ -1567,7 +1570,7 @@
     <numFmt numFmtId="164" formatCode="h&quot;:&quot;mm"/>
     <numFmt numFmtId="165" formatCode="[$Rp]#,##0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1593,6 +1596,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1692,10 +1702,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1760,8 +1771,10 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1977,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="43" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2834,7 +2847,7 @@
       <c r="M16" s="11">
         <v>113.124476949129</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N16" s="24" t="s">
         <v>423</v>
       </c>
       <c r="O16" s="1"/>
@@ -2940,8 +2953,8 @@
       <c r="M18" s="11">
         <v>112.813400050927</v>
       </c>
-      <c r="N18" s="12" t="s">
-        <v>424</v>
+      <c r="N18" s="24" t="s">
+        <v>509</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -29006,7 +29019,11 @@
       <c r="L1000" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N18" r:id="rId1" xr:uid="{70BF9E74-6CF9-4BA2-9074-210AF0782F68}"/>
+    <hyperlink ref="N16" r:id="rId2" xr:uid="{0098AFA4-C3CA-406D-B16C-BD7DA56E5F53}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>